<commit_message>
fixed condition files, added stimuli for green_purple_orange
</commit_message>
<xml_diff>
--- a/green_orange_purple/Condition_File_green_orange_purple.xlsx
+++ b/green_orange_purple/Condition_File_green_orange_purple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rochellekaper/Desktop/Both_Tasks/green_orange_purple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747D4D5D-6DC4-5348-B2AD-BB89A6A5DD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E943C8-FC97-C94A-BB70-5996273416F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="5480" windowWidth="29400" windowHeight="18380" xr2:uid="{50BE362F-E7B0-5840-BBD3-B85E4770FAD8}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="13160" xr2:uid="{50BE362F-E7B0-5840-BBD3-B85E4770FAD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4470,7 +4470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4486,9 +4486,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4807,9 +4804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4763C67E-82ED-7748-9439-DB0637206C14}">
   <dimension ref="A1:M301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="68" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D142" sqref="D142"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="68" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F304" sqref="F304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -4882,7 +4879,7 @@
       <c r="D2" s="1" t="s">
         <v>1231</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1">
@@ -4923,7 +4920,7 @@
       <c r="D3" s="1" t="s">
         <v>1232</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="1">
@@ -4964,7 +4961,7 @@
       <c r="D4" s="6" t="s">
         <v>1233</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="1">
@@ -5005,7 +5002,7 @@
       <c r="D5" s="4" t="s">
         <v>1234</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="1">
@@ -5046,7 +5043,7 @@
       <c r="D6" s="4" t="s">
         <v>1235</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="1">
@@ -5087,7 +5084,7 @@
       <c r="D7" s="1" t="s">
         <v>1257</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="1">
@@ -5128,7 +5125,7 @@
       <c r="D8" s="1" t="s">
         <v>1259</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="1">
@@ -5169,7 +5166,7 @@
       <c r="D9" s="1" t="s">
         <v>1261</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="1">
@@ -5210,7 +5207,7 @@
       <c r="D10" s="1" t="s">
         <v>1263</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="1">
@@ -5251,7 +5248,7 @@
       <c r="D11" s="1" t="s">
         <v>1265</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="1">
@@ -5292,7 +5289,7 @@
       <c r="D12" s="1" t="s">
         <v>1267</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="1">
@@ -5333,7 +5330,7 @@
       <c r="D13" s="1" t="s">
         <v>1269</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="1">
@@ -5374,7 +5371,7 @@
       <c r="D14" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="1">
@@ -5415,7 +5412,7 @@
       <c r="D15" s="1" t="s">
         <v>1272</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="1">
@@ -5456,7 +5453,7 @@
       <c r="D16" s="1" t="s">
         <v>1274</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="1">
@@ -5497,7 +5494,7 @@
       <c r="D17" s="1" t="s">
         <v>1302</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="1">
@@ -5538,7 +5535,7 @@
       <c r="D18" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="1">
@@ -5579,7 +5576,7 @@
       <c r="D19" s="1" t="s">
         <v>1306</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="1">
@@ -5620,7 +5617,7 @@
       <c r="D20" s="1" t="s">
         <v>1308</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="1">
@@ -5661,7 +5658,7 @@
       <c r="D21" s="1" t="s">
         <v>1310</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="1">
@@ -5702,7 +5699,7 @@
       <c r="D22" s="1" t="s">
         <v>1312</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="1">
@@ -5743,7 +5740,7 @@
       <c r="D23" s="1" t="s">
         <v>1314</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>17</v>
       </c>
       <c r="F23" s="1">
@@ -5784,7 +5781,7 @@
       <c r="D24" s="1" t="s">
         <v>1316</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>17</v>
       </c>
       <c r="F24" s="1">
@@ -5825,7 +5822,7 @@
       <c r="D25" s="1" t="s">
         <v>1318</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="1">
@@ -5866,7 +5863,7 @@
       <c r="D26" s="1" t="s">
         <v>1320</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>16</v>
       </c>
       <c r="F26" s="1">
@@ -5907,7 +5904,7 @@
       <c r="D27" s="1" t="s">
         <v>1335</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>16</v>
       </c>
       <c r="F27" s="1">
@@ -5948,7 +5945,7 @@
       <c r="D28" s="1" t="s">
         <v>1336</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="1">
@@ -5989,7 +5986,7 @@
       <c r="D29" s="1" t="s">
         <v>1337</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>16</v>
       </c>
       <c r="F29" s="1">
@@ -6030,7 +6027,7 @@
       <c r="D30" s="1" t="s">
         <v>1338</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="1">
@@ -6071,7 +6068,7 @@
       <c r="D31" s="1" t="s">
         <v>1339</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>17</v>
       </c>
       <c r="F31" s="1">
@@ -6112,7 +6109,7 @@
       <c r="D32" s="1" t="s">
         <v>1340</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>17</v>
       </c>
       <c r="F32" s="1">
@@ -6153,7 +6150,7 @@
       <c r="D33" s="1" t="s">
         <v>1341</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>17</v>
       </c>
       <c r="F33" s="1">
@@ -6194,7 +6191,7 @@
       <c r="D34" s="1" t="s">
         <v>1342</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="1">
@@ -6235,7 +6232,7 @@
       <c r="D35" s="1" t="s">
         <v>1343</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>16</v>
       </c>
       <c r="F35" s="1">
@@ -6276,7 +6273,7 @@
       <c r="D36" s="1" t="s">
         <v>1344</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>16</v>
       </c>
       <c r="F36" s="1">
@@ -6317,7 +6314,7 @@
       <c r="D37" s="1" t="s">
         <v>1345</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>16</v>
       </c>
       <c r="F37" s="1">
@@ -6358,7 +6355,7 @@
       <c r="D38" s="1" t="s">
         <v>1346</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>17</v>
       </c>
       <c r="F38" s="1">
@@ -6399,7 +6396,7 @@
       <c r="D39" s="1" t="s">
         <v>1347</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>17</v>
       </c>
       <c r="F39" s="1">
@@ -6440,7 +6437,7 @@
       <c r="D40" s="1" t="s">
         <v>1348</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>17</v>
       </c>
       <c r="F40" s="1">
@@ -6481,7 +6478,7 @@
       <c r="D41" s="1" t="s">
         <v>1349</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>17</v>
       </c>
       <c r="F41" s="1">
@@ -6522,7 +6519,7 @@
       <c r="D42" s="1" t="s">
         <v>1350</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>16</v>
       </c>
       <c r="F42" s="1">
@@ -6563,7 +6560,7 @@
       <c r="D43" s="1" t="s">
         <v>1351</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>16</v>
       </c>
       <c r="F43" s="1">
@@ -6604,7 +6601,7 @@
       <c r="D44" s="1" t="s">
         <v>1352</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>16</v>
       </c>
       <c r="F44" s="1">
@@ -6645,7 +6642,7 @@
       <c r="D45" s="1" t="s">
         <v>1353</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>16</v>
       </c>
       <c r="F45" s="1">
@@ -6686,7 +6683,7 @@
       <c r="D46" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>17</v>
       </c>
       <c r="F46" s="1">
@@ -6727,7 +6724,7 @@
       <c r="D47" s="1" t="s">
         <v>1374</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>17</v>
       </c>
       <c r="F47" s="1">
@@ -6768,7 +6765,7 @@
       <c r="D48" s="1" t="s">
         <v>1375</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>17</v>
       </c>
       <c r="F48" s="1">
@@ -6809,7 +6806,7 @@
       <c r="D49" s="1" t="s">
         <v>1376</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>17</v>
       </c>
       <c r="F49" s="1">
@@ -6850,7 +6847,7 @@
       <c r="D50" s="1" t="s">
         <v>1377</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>16</v>
       </c>
       <c r="F50" s="1">
@@ -6891,7 +6888,7 @@
       <c r="D51" s="1" t="s">
         <v>1378</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>16</v>
       </c>
       <c r="F51" s="1">
@@ -6932,7 +6929,7 @@
       <c r="D52" s="1" t="s">
         <v>1380</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>16</v>
       </c>
       <c r="F52" s="1">
@@ -6973,7 +6970,7 @@
       <c r="D53" s="1" t="s">
         <v>1382</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>16</v>
       </c>
       <c r="F53" s="1">
@@ -7014,7 +7011,7 @@
       <c r="D54" s="1" t="s">
         <v>1383</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" t="s">
         <v>17</v>
       </c>
       <c r="F54" s="1">
@@ -7055,7 +7052,7 @@
       <c r="D55" s="1" t="s">
         <v>1384</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" t="s">
         <v>17</v>
       </c>
       <c r="F55" s="1">
@@ -7096,7 +7093,7 @@
       <c r="D56" s="1" t="s">
         <v>1385</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>17</v>
       </c>
       <c r="F56" s="1">
@@ -7137,7 +7134,7 @@
       <c r="D57" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>17</v>
       </c>
       <c r="F57" s="1">
@@ -7178,7 +7175,7 @@
       <c r="D58" s="1" t="s">
         <v>1400</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" t="s">
         <v>16</v>
       </c>
       <c r="F58" s="1">
@@ -7219,7 +7216,7 @@
       <c r="D59" s="1" t="s">
         <v>1401</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" t="s">
         <v>16</v>
       </c>
       <c r="F59" s="1">
@@ -7260,7 +7257,7 @@
       <c r="D60" s="1" t="s">
         <v>1402</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>16</v>
       </c>
       <c r="F60" s="1">
@@ -7301,7 +7298,7 @@
       <c r="D61" s="1" t="s">
         <v>1403</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" t="s">
         <v>16</v>
       </c>
       <c r="F61" s="1">
@@ -7342,7 +7339,7 @@
       <c r="D62" s="1" t="s">
         <v>1404</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" t="s">
         <v>17</v>
       </c>
       <c r="F62" s="1">
@@ -7383,7 +7380,7 @@
       <c r="D63" s="1" t="s">
         <v>1405</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" t="s">
         <v>17</v>
       </c>
       <c r="F63" s="1">
@@ -7424,7 +7421,7 @@
       <c r="D64" s="1" t="s">
         <v>1406</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>17</v>
       </c>
       <c r="F64" s="1">
@@ -7465,7 +7462,7 @@
       <c r="D65" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" t="s">
         <v>17</v>
       </c>
       <c r="F65" s="1">
@@ -7506,7 +7503,7 @@
       <c r="D66" s="1" t="s">
         <v>1407</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" t="s">
         <v>16</v>
       </c>
       <c r="F66" s="1">
@@ -7547,7 +7544,7 @@
       <c r="D67" s="1" t="s">
         <v>1418</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" t="s">
         <v>16</v>
       </c>
       <c r="F67" s="1">
@@ -7588,7 +7585,7 @@
       <c r="D68" s="1" t="s">
         <v>1420</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" t="s">
         <v>16</v>
       </c>
       <c r="F68" s="1">
@@ -7629,7 +7626,7 @@
       <c r="D69" s="1" t="s">
         <v>1422</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>16</v>
       </c>
       <c r="F69" s="1">
@@ -7670,7 +7667,7 @@
       <c r="D70" s="1" t="s">
         <v>1424</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" t="s">
         <v>17</v>
       </c>
       <c r="F70" s="1">
@@ -7711,7 +7708,7 @@
       <c r="D71" s="1" t="s">
         <v>1426</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" t="s">
         <v>17</v>
       </c>
       <c r="F71" s="1">
@@ -7752,7 +7749,7 @@
       <c r="D72" s="1" t="s">
         <v>1431</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" t="s">
         <v>17</v>
       </c>
       <c r="F72" s="1">
@@ -7793,8 +7790,8 @@
       <c r="D73" s="1" t="s">
         <v>1433</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>17</v>
+      <c r="E73" t="s">
+        <v>16</v>
       </c>
       <c r="F73" s="1">
         <v>0.25</v>
@@ -7834,7 +7831,7 @@
       <c r="D74" s="1" t="s">
         <v>1435</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" t="s">
         <v>16</v>
       </c>
       <c r="F74" s="1">
@@ -7875,7 +7872,7 @@
       <c r="D75" s="1" t="s">
         <v>1437</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" t="s">
         <v>16</v>
       </c>
       <c r="F75" s="1">
@@ -7916,7 +7913,7 @@
       <c r="D76" s="1" t="s">
         <v>1439</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" t="s">
         <v>16</v>
       </c>
       <c r="F76" s="1">
@@ -7957,7 +7954,7 @@
       <c r="D77" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" t="s">
         <v>16</v>
       </c>
       <c r="F77" s="1">
@@ -7998,8 +7995,8 @@
       <c r="D78" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>17</v>
+      <c r="E78" t="s">
+        <v>16</v>
       </c>
       <c r="F78" s="1">
         <v>-0.25</v>
@@ -8039,8 +8036,8 @@
       <c r="D79" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>17</v>
+      <c r="E79" t="s">
+        <v>16</v>
       </c>
       <c r="F79" s="1">
         <v>-0.25</v>
@@ -8080,8 +8077,8 @@
       <c r="D80" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>17</v>
+      <c r="E80" t="s">
+        <v>16</v>
       </c>
       <c r="F80" s="1">
         <v>-0.25</v>
@@ -8121,8 +8118,8 @@
       <c r="D81" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E81" s="1" t="s">
-        <v>17</v>
+      <c r="E81" t="s">
+        <v>16</v>
       </c>
       <c r="F81" s="1">
         <v>-0.25</v>
@@ -8162,7 +8159,7 @@
       <c r="D82" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E82" t="s">
         <v>16</v>
       </c>
       <c r="F82" s="1">
@@ -8203,7 +8200,7 @@
       <c r="D83" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" t="s">
         <v>16</v>
       </c>
       <c r="F83" s="1">
@@ -8244,7 +8241,7 @@
       <c r="D84" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" t="s">
         <v>16</v>
       </c>
       <c r="F84" s="1">
@@ -8285,7 +8282,7 @@
       <c r="D85" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E85" t="s">
         <v>16</v>
       </c>
       <c r="F85" s="1">
@@ -8326,8 +8323,8 @@
       <c r="D86" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>17</v>
+      <c r="E86" t="s">
+        <v>16</v>
       </c>
       <c r="F86" s="1">
         <v>-0.25</v>
@@ -8367,8 +8364,8 @@
       <c r="D87" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>17</v>
+      <c r="E87" t="s">
+        <v>16</v>
       </c>
       <c r="F87" s="1">
         <v>-0.25</v>
@@ -8408,8 +8405,8 @@
       <c r="D88" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>17</v>
+      <c r="E88" t="s">
+        <v>16</v>
       </c>
       <c r="F88" s="1">
         <v>-0.25</v>
@@ -8449,8 +8446,8 @@
       <c r="D89" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>17</v>
+      <c r="E89" t="s">
+        <v>16</v>
       </c>
       <c r="F89" s="1">
         <v>-0.25</v>
@@ -8490,7 +8487,7 @@
       <c r="D90" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E90" t="s">
         <v>16</v>
       </c>
       <c r="F90" s="1">
@@ -8531,7 +8528,7 @@
       <c r="D91" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" t="s">
         <v>16</v>
       </c>
       <c r="F91" s="1">
@@ -8572,7 +8569,7 @@
       <c r="D92" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E92" t="s">
         <v>16</v>
       </c>
       <c r="F92" s="1">
@@ -8613,7 +8610,7 @@
       <c r="D93" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E93" t="s">
         <v>16</v>
       </c>
       <c r="F93" s="1">
@@ -8654,8 +8651,8 @@
       <c r="D94" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E94" s="1" t="s">
-        <v>17</v>
+      <c r="E94" t="s">
+        <v>16</v>
       </c>
       <c r="F94" s="1">
         <v>-0.25</v>
@@ -8695,8 +8692,8 @@
       <c r="D95" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>17</v>
+      <c r="E95" t="s">
+        <v>16</v>
       </c>
       <c r="F95" s="1">
         <v>-0.25</v>
@@ -8736,8 +8733,8 @@
       <c r="D96" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>17</v>
+      <c r="E96" t="s">
+        <v>16</v>
       </c>
       <c r="F96" s="1">
         <v>-0.25</v>
@@ -8777,8 +8774,8 @@
       <c r="D97" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>17</v>
+      <c r="E97" t="s">
+        <v>16</v>
       </c>
       <c r="F97" s="1">
         <v>-0.25</v>
@@ -8818,7 +8815,7 @@
       <c r="D98" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E98" t="s">
         <v>16</v>
       </c>
       <c r="F98" s="1">
@@ -8859,7 +8856,7 @@
       <c r="D99" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E99" t="s">
         <v>16</v>
       </c>
       <c r="F99" s="1">
@@ -8900,7 +8897,7 @@
       <c r="D100" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E100" t="s">
         <v>16</v>
       </c>
       <c r="F100" s="1">
@@ -8941,7 +8938,7 @@
       <c r="D101" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E101" t="s">
         <v>16</v>
       </c>
       <c r="F101" s="1">
@@ -8982,8 +8979,8 @@
       <c r="D102" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>17</v>
+      <c r="E102" t="s">
+        <v>16</v>
       </c>
       <c r="F102" s="1">
         <v>-0.25</v>
@@ -9023,8 +9020,8 @@
       <c r="D103" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="E103" s="1" t="s">
-        <v>17</v>
+      <c r="E103" t="s">
+        <v>16</v>
       </c>
       <c r="F103" s="1">
         <v>-0.25</v>
@@ -9064,8 +9061,8 @@
       <c r="D104" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="E104" s="1" t="s">
-        <v>17</v>
+      <c r="E104" t="s">
+        <v>16</v>
       </c>
       <c r="F104" s="1">
         <v>-0.25</v>
@@ -9105,8 +9102,8 @@
       <c r="D105" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="E105" s="1" t="s">
-        <v>17</v>
+      <c r="E105" t="s">
+        <v>16</v>
       </c>
       <c r="F105" s="1">
         <v>-0.25</v>
@@ -9146,7 +9143,7 @@
       <c r="D106" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="E106" t="s">
         <v>16</v>
       </c>
       <c r="F106" s="1">
@@ -9187,7 +9184,7 @@
       <c r="D107" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="E107" t="s">
         <v>16</v>
       </c>
       <c r="F107" s="1">
@@ -9228,7 +9225,7 @@
       <c r="D108" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="E108" t="s">
         <v>16</v>
       </c>
       <c r="F108" s="1">
@@ -9269,7 +9266,7 @@
       <c r="D109" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="E109" t="s">
         <v>16</v>
       </c>
       <c r="F109" s="1">
@@ -9310,8 +9307,8 @@
       <c r="D110" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>17</v>
+      <c r="E110" t="s">
+        <v>16</v>
       </c>
       <c r="F110" s="1">
         <v>-0.25</v>
@@ -9351,8 +9348,8 @@
       <c r="D111" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>17</v>
+      <c r="E111" t="s">
+        <v>16</v>
       </c>
       <c r="F111" s="1">
         <v>-0.25</v>
@@ -9392,8 +9389,8 @@
       <c r="D112" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>17</v>
+      <c r="E112" t="s">
+        <v>16</v>
       </c>
       <c r="F112" s="1">
         <v>-0.25</v>
@@ -9433,8 +9430,8 @@
       <c r="D113" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="E113" s="1" t="s">
-        <v>17</v>
+      <c r="E113" t="s">
+        <v>16</v>
       </c>
       <c r="F113" s="1">
         <v>-0.25</v>
@@ -9474,7 +9471,7 @@
       <c r="D114" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E114" s="1" t="s">
+      <c r="E114" t="s">
         <v>16</v>
       </c>
       <c r="F114" s="1">
@@ -9515,7 +9512,7 @@
       <c r="D115" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E115" t="s">
         <v>16</v>
       </c>
       <c r="F115" s="1">
@@ -9556,7 +9553,7 @@
       <c r="D116" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E116" s="1" t="s">
+      <c r="E116" t="s">
         <v>16</v>
       </c>
       <c r="F116" s="1">
@@ -9597,7 +9594,7 @@
       <c r="D117" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E117" s="1" t="s">
+      <c r="E117" t="s">
         <v>16</v>
       </c>
       <c r="F117" s="1">
@@ -9638,8 +9635,8 @@
       <c r="D118" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="E118" s="1" t="s">
-        <v>17</v>
+      <c r="E118" t="s">
+        <v>16</v>
       </c>
       <c r="F118" s="1">
         <v>-0.25</v>
@@ -9679,8 +9676,8 @@
       <c r="D119" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>17</v>
+      <c r="E119" t="s">
+        <v>16</v>
       </c>
       <c r="F119" s="1">
         <v>-0.25</v>
@@ -9720,8 +9717,8 @@
       <c r="D120" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>17</v>
+      <c r="E120" t="s">
+        <v>16</v>
       </c>
       <c r="F120" s="1">
         <v>-0.25</v>
@@ -9761,8 +9758,8 @@
       <c r="D121" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="E121" s="1" t="s">
-        <v>17</v>
+      <c r="E121" t="s">
+        <v>16</v>
       </c>
       <c r="F121" s="1">
         <v>-0.25</v>
@@ -9802,7 +9799,7 @@
       <c r="D122" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="E122" t="s">
         <v>16</v>
       </c>
       <c r="F122" s="1">
@@ -9843,7 +9840,7 @@
       <c r="D123" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="E123" s="1" t="s">
+      <c r="E123" t="s">
         <v>16</v>
       </c>
       <c r="F123" s="1">
@@ -9884,7 +9881,7 @@
       <c r="D124" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E124" s="1" t="s">
+      <c r="E124" t="s">
         <v>16</v>
       </c>
       <c r="F124" s="1">
@@ -9925,7 +9922,7 @@
       <c r="D125" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E125" s="1" t="s">
+      <c r="E125" t="s">
         <v>16</v>
       </c>
       <c r="F125" s="1">
@@ -9966,8 +9963,8 @@
       <c r="D126" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="E126" s="1" t="s">
-        <v>17</v>
+      <c r="E126" t="s">
+        <v>16</v>
       </c>
       <c r="F126" s="1">
         <v>-0.25</v>
@@ -10007,8 +10004,8 @@
       <c r="D127" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>17</v>
+      <c r="E127" t="s">
+        <v>16</v>
       </c>
       <c r="F127" s="1">
         <v>-0.25</v>
@@ -10048,8 +10045,8 @@
       <c r="D128" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E128" s="1" t="s">
-        <v>17</v>
+      <c r="E128" t="s">
+        <v>16</v>
       </c>
       <c r="F128" s="1">
         <v>-0.25</v>
@@ -10089,8 +10086,8 @@
       <c r="D129" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="E129" s="1" t="s">
-        <v>17</v>
+      <c r="E129" t="s">
+        <v>16</v>
       </c>
       <c r="F129" s="1">
         <v>-0.25</v>
@@ -10130,7 +10127,7 @@
       <c r="D130" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E130" s="1" t="s">
+      <c r="E130" t="s">
         <v>16</v>
       </c>
       <c r="F130" s="1">
@@ -10171,7 +10168,7 @@
       <c r="D131" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="E131" s="1" t="s">
+      <c r="E131" t="s">
         <v>16</v>
       </c>
       <c r="F131" s="1">
@@ -10212,7 +10209,7 @@
       <c r="D132" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E132" s="1" t="s">
+      <c r="E132" t="s">
         <v>16</v>
       </c>
       <c r="F132" s="1">
@@ -10253,7 +10250,7 @@
       <c r="D133" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E133" s="1" t="s">
+      <c r="E133" t="s">
         <v>16</v>
       </c>
       <c r="F133" s="1">
@@ -10294,8 +10291,8 @@
       <c r="D134" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E134" s="1" t="s">
-        <v>17</v>
+      <c r="E134" t="s">
+        <v>16</v>
       </c>
       <c r="F134" s="1">
         <v>-0.25</v>
@@ -10335,8 +10332,8 @@
       <c r="D135" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E135" s="1" t="s">
-        <v>17</v>
+      <c r="E135" t="s">
+        <v>16</v>
       </c>
       <c r="F135" s="1">
         <v>-0.25</v>
@@ -10376,8 +10373,8 @@
       <c r="D136" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="E136" s="1" t="s">
-        <v>17</v>
+      <c r="E136" t="s">
+        <v>16</v>
       </c>
       <c r="F136" s="1">
         <v>-0.25</v>
@@ -10417,8 +10414,8 @@
       <c r="D137" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="E137" s="1" t="s">
-        <v>17</v>
+      <c r="E137" t="s">
+        <v>16</v>
       </c>
       <c r="F137" s="1">
         <v>-0.25</v>
@@ -10458,7 +10455,7 @@
       <c r="D138" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="E138" s="1" t="s">
+      <c r="E138" t="s">
         <v>16</v>
       </c>
       <c r="F138" s="1">
@@ -10499,7 +10496,7 @@
       <c r="D139" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E139" s="1" t="s">
+      <c r="E139" t="s">
         <v>16</v>
       </c>
       <c r="F139" s="1">
@@ -10540,7 +10537,7 @@
       <c r="D140" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="E140" s="1" t="s">
+      <c r="E140" t="s">
         <v>16</v>
       </c>
       <c r="F140" s="1">
@@ -10581,7 +10578,7 @@
       <c r="D141" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="E141" s="1" t="s">
+      <c r="E141" t="s">
         <v>16</v>
       </c>
       <c r="F141" s="1">
@@ -10616,14 +10613,14 @@
       <c r="B142" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="C142" s="7" t="s">
+      <c r="C142" s="1" t="s">
         <v>1456</v>
       </c>
-      <c r="D142" s="7" t="s">
+      <c r="D142" s="1" t="s">
         <v>1457</v>
       </c>
-      <c r="E142" s="1" t="s">
-        <v>17</v>
+      <c r="E142" t="s">
+        <v>16</v>
       </c>
       <c r="F142" s="1">
         <v>-0.25</v>
@@ -10663,8 +10660,8 @@
       <c r="D143" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="E143" s="1" t="s">
-        <v>17</v>
+      <c r="E143" t="s">
+        <v>16</v>
       </c>
       <c r="F143" s="1">
         <v>-0.25</v>
@@ -10704,8 +10701,8 @@
       <c r="D144" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="E144" s="1" t="s">
-        <v>17</v>
+      <c r="E144" t="s">
+        <v>16</v>
       </c>
       <c r="F144" s="1">
         <v>-0.25</v>
@@ -10745,8 +10742,8 @@
       <c r="D145" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="E145" s="1" t="s">
-        <v>17</v>
+      <c r="E145" t="s">
+        <v>16</v>
       </c>
       <c r="F145" s="1">
         <v>-0.25</v>
@@ -10786,7 +10783,7 @@
       <c r="D146" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="E146" s="1" t="s">
+      <c r="E146" t="s">
         <v>16</v>
       </c>
       <c r="F146" s="1">
@@ -10827,7 +10824,7 @@
       <c r="D147" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="E147" s="1" t="s">
+      <c r="E147" t="s">
         <v>16</v>
       </c>
       <c r="F147" s="1">
@@ -10868,7 +10865,7 @@
       <c r="D148" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E148" s="1" t="s">
+      <c r="E148" t="s">
         <v>16</v>
       </c>
       <c r="F148" s="1">
@@ -10909,7 +10906,7 @@
       <c r="D149" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="E149" s="1" t="s">
+      <c r="E149" t="s">
         <v>16</v>
       </c>
       <c r="F149" s="1">
@@ -10950,8 +10947,8 @@
       <c r="D150" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="E150" s="1" t="s">
-        <v>17</v>
+      <c r="E150" t="s">
+        <v>16</v>
       </c>
       <c r="F150" s="1">
         <v>-0.25</v>
@@ -10991,8 +10988,8 @@
       <c r="D151" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="E151" s="1" t="s">
-        <v>17</v>
+      <c r="E151" t="s">
+        <v>16</v>
       </c>
       <c r="F151" s="1">
         <v>-0.25</v>
@@ -11032,8 +11029,8 @@
       <c r="D152" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="E152" s="1" t="s">
-        <v>17</v>
+      <c r="E152" t="s">
+        <v>16</v>
       </c>
       <c r="F152" s="1">
         <v>-0.25</v>
@@ -11073,8 +11070,8 @@
       <c r="D153" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="E153" s="1" t="s">
-        <v>17</v>
+      <c r="E153" t="s">
+        <v>16</v>
       </c>
       <c r="F153" s="1">
         <v>-0.25</v>
@@ -11114,7 +11111,7 @@
       <c r="D154" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="E154" s="1" t="s">
+      <c r="E154" t="s">
         <v>16</v>
       </c>
       <c r="F154" s="1">
@@ -11155,7 +11152,7 @@
       <c r="D155" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E155" s="1" t="s">
+      <c r="E155" t="s">
         <v>16</v>
       </c>
       <c r="F155" s="1">
@@ -11196,7 +11193,7 @@
       <c r="D156" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E156" s="1" t="s">
+      <c r="E156" t="s">
         <v>16</v>
       </c>
       <c r="F156" s="1">
@@ -11237,7 +11234,7 @@
       <c r="D157" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="E157" s="1" t="s">
+      <c r="E157" t="s">
         <v>16</v>
       </c>
       <c r="F157" s="1">
@@ -11278,8 +11275,8 @@
       <c r="D158" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="E158" s="1" t="s">
-        <v>17</v>
+      <c r="E158" t="s">
+        <v>16</v>
       </c>
       <c r="F158" s="1">
         <v>-0.25</v>
@@ -11319,8 +11316,8 @@
       <c r="D159" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="E159" s="1" t="s">
-        <v>17</v>
+      <c r="E159" t="s">
+        <v>16</v>
       </c>
       <c r="F159" s="1">
         <v>-0.25</v>
@@ -11360,8 +11357,8 @@
       <c r="D160" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="E160" s="1" t="s">
-        <v>17</v>
+      <c r="E160" t="s">
+        <v>16</v>
       </c>
       <c r="F160" s="1">
         <v>-0.25</v>
@@ -11401,8 +11398,8 @@
       <c r="D161" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="E161" s="1" t="s">
-        <v>17</v>
+      <c r="E161" t="s">
+        <v>16</v>
       </c>
       <c r="F161" s="1">
         <v>-0.25</v>
@@ -11442,7 +11439,7 @@
       <c r="D162" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="E162" s="1" t="s">
+      <c r="E162" t="s">
         <v>16</v>
       </c>
       <c r="F162" s="1">
@@ -11483,7 +11480,7 @@
       <c r="D163" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="E163" s="1" t="s">
+      <c r="E163" t="s">
         <v>16</v>
       </c>
       <c r="F163" s="1">
@@ -11524,7 +11521,7 @@
       <c r="D164" s="1" t="s">
         <v>1226</v>
       </c>
-      <c r="E164" s="1" t="s">
+      <c r="E164" t="s">
         <v>16</v>
       </c>
       <c r="F164" s="1">
@@ -11565,7 +11562,7 @@
       <c r="D165" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="E165" s="1" t="s">
+      <c r="E165" t="s">
         <v>16</v>
       </c>
       <c r="F165" s="1">
@@ -11600,14 +11597,14 @@
       <c r="B166" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="C166" s="7" t="s">
+      <c r="C166" s="1" t="s">
         <v>1454</v>
       </c>
-      <c r="D166" s="7" t="s">
+      <c r="D166" s="1" t="s">
         <v>1455</v>
       </c>
-      <c r="E166" s="1" t="s">
-        <v>17</v>
+      <c r="E166" t="s">
+        <v>16</v>
       </c>
       <c r="F166" s="1">
         <v>-0.25</v>
@@ -11647,8 +11644,8 @@
       <c r="D167" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="E167" s="1" t="s">
-        <v>17</v>
+      <c r="E167" t="s">
+        <v>16</v>
       </c>
       <c r="F167" s="1">
         <v>-0.25</v>
@@ -11688,8 +11685,8 @@
       <c r="D168" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E168" s="1" t="s">
-        <v>17</v>
+      <c r="E168" t="s">
+        <v>16</v>
       </c>
       <c r="F168" s="1">
         <v>-0.25</v>
@@ -11729,8 +11726,8 @@
       <c r="D169" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="E169" s="1" t="s">
-        <v>17</v>
+      <c r="E169" t="s">
+        <v>16</v>
       </c>
       <c r="F169" s="1">
         <v>-0.25</v>
@@ -11770,7 +11767,7 @@
       <c r="D170" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="E170" s="1" t="s">
+      <c r="E170" t="s">
         <v>16</v>
       </c>
       <c r="F170" s="1">
@@ -11811,7 +11808,7 @@
       <c r="D171" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="E171" s="1" t="s">
+      <c r="E171" t="s">
         <v>16</v>
       </c>
       <c r="F171" s="1">
@@ -11852,7 +11849,7 @@
       <c r="D172" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="E172" s="1" t="s">
+      <c r="E172" t="s">
         <v>16</v>
       </c>
       <c r="F172" s="1">
@@ -11893,7 +11890,7 @@
       <c r="D173" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E173" s="1" t="s">
+      <c r="E173" t="s">
         <v>16</v>
       </c>
       <c r="F173" s="1">
@@ -11934,8 +11931,8 @@
       <c r="D174" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="E174" s="1" t="s">
-        <v>17</v>
+      <c r="E174" t="s">
+        <v>16</v>
       </c>
       <c r="F174" s="1">
         <v>-0.25</v>
@@ -11975,8 +11972,8 @@
       <c r="D175" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="E175" s="1" t="s">
-        <v>17</v>
+      <c r="E175" t="s">
+        <v>16</v>
       </c>
       <c r="F175" s="1">
         <v>-0.25</v>
@@ -12016,8 +12013,8 @@
       <c r="D176" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="E176" s="1" t="s">
-        <v>17</v>
+      <c r="E176" t="s">
+        <v>16</v>
       </c>
       <c r="F176" s="1">
         <v>-0.25</v>
@@ -12057,8 +12054,8 @@
       <c r="D177" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="E177" s="1" t="s">
-        <v>17</v>
+      <c r="E177" t="s">
+        <v>16</v>
       </c>
       <c r="F177" s="1">
         <v>-0.25</v>
@@ -12098,7 +12095,7 @@
       <c r="D178" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="E178" s="1" t="s">
+      <c r="E178" t="s">
         <v>16</v>
       </c>
       <c r="F178" s="1">
@@ -12139,7 +12136,7 @@
       <c r="D179" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="E179" s="1" t="s">
+      <c r="E179" t="s">
         <v>16</v>
       </c>
       <c r="F179" s="1">
@@ -12180,7 +12177,7 @@
       <c r="D180" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="E180" s="1" t="s">
+      <c r="E180" t="s">
         <v>16</v>
       </c>
       <c r="F180" s="1">
@@ -12221,7 +12218,7 @@
       <c r="D181" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="E181" s="1" t="s">
+      <c r="E181" t="s">
         <v>16</v>
       </c>
       <c r="F181" s="1">
@@ -12262,8 +12259,8 @@
       <c r="D182" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="E182" s="1" t="s">
-        <v>17</v>
+      <c r="E182" t="s">
+        <v>16</v>
       </c>
       <c r="F182" s="1">
         <v>-0.25</v>
@@ -12303,8 +12300,8 @@
       <c r="D183" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="E183" s="1" t="s">
-        <v>17</v>
+      <c r="E183" t="s">
+        <v>16</v>
       </c>
       <c r="F183" s="1">
         <v>-0.25</v>
@@ -12344,8 +12341,8 @@
       <c r="D184" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="E184" s="1" t="s">
-        <v>17</v>
+      <c r="E184" t="s">
+        <v>16</v>
       </c>
       <c r="F184" s="1">
         <v>-0.25</v>
@@ -12385,8 +12382,8 @@
       <c r="D185" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="E185" s="1" t="s">
-        <v>17</v>
+      <c r="E185" t="s">
+        <v>16</v>
       </c>
       <c r="F185" s="1">
         <v>-0.25</v>
@@ -12426,7 +12423,7 @@
       <c r="D186" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="E186" s="1" t="s">
+      <c r="E186" t="s">
         <v>16</v>
       </c>
       <c r="F186" s="1">
@@ -12467,7 +12464,7 @@
       <c r="D187" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="E187" s="1" t="s">
+      <c r="E187" t="s">
         <v>16</v>
       </c>
       <c r="F187" s="1">
@@ -12508,7 +12505,7 @@
       <c r="D188" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E188" s="1" t="s">
+      <c r="E188" t="s">
         <v>16</v>
       </c>
       <c r="F188" s="1">
@@ -12549,7 +12546,7 @@
       <c r="D189" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="E189" s="1" t="s">
+      <c r="E189" t="s">
         <v>16</v>
       </c>
       <c r="F189" s="1">
@@ -12590,7 +12587,7 @@
       <c r="D190" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="E190" s="1" t="s">
+      <c r="E190" t="s">
         <v>17</v>
       </c>
       <c r="F190" s="1">
@@ -12631,7 +12628,7 @@
       <c r="D191" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E191" s="1" t="s">
+      <c r="E191" t="s">
         <v>17</v>
       </c>
       <c r="F191" s="1">
@@ -12672,7 +12669,7 @@
       <c r="D192" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="E192" s="1" t="s">
+      <c r="E192" t="s">
         <v>17</v>
       </c>
       <c r="F192" s="1">
@@ -12713,7 +12710,7 @@
       <c r="D193" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="E193" s="1" t="s">
+      <c r="E193" t="s">
         <v>17</v>
       </c>
       <c r="F193" s="1">
@@ -12754,8 +12751,8 @@
       <c r="D194" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="E194" s="1" t="s">
-        <v>16</v>
+      <c r="E194" t="s">
+        <v>17</v>
       </c>
       <c r="F194" s="1">
         <v>0.25</v>
@@ -12795,8 +12792,8 @@
       <c r="D195" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="E195" s="1" t="s">
-        <v>16</v>
+      <c r="E195" t="s">
+        <v>17</v>
       </c>
       <c r="F195" s="1">
         <v>0.25</v>
@@ -12836,8 +12833,8 @@
       <c r="D196" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E196" s="1" t="s">
-        <v>16</v>
+      <c r="E196" t="s">
+        <v>17</v>
       </c>
       <c r="F196" s="1">
         <v>0.25</v>
@@ -12877,8 +12874,8 @@
       <c r="D197" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="E197" s="1" t="s">
-        <v>16</v>
+      <c r="E197" t="s">
+        <v>17</v>
       </c>
       <c r="F197" s="1">
         <v>0.25</v>
@@ -12918,7 +12915,7 @@
       <c r="D198" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="E198" s="1" t="s">
+      <c r="E198" t="s">
         <v>17</v>
       </c>
       <c r="F198" s="1">
@@ -12959,7 +12956,7 @@
       <c r="D199" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="E199" s="1" t="s">
+      <c r="E199" t="s">
         <v>17</v>
       </c>
       <c r="F199" s="1">
@@ -13000,7 +12997,7 @@
       <c r="D200" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="E200" s="1" t="s">
+      <c r="E200" t="s">
         <v>17</v>
       </c>
       <c r="F200" s="1">
@@ -13041,7 +13038,7 @@
       <c r="D201" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="E201" s="1" t="s">
+      <c r="E201" t="s">
         <v>17</v>
       </c>
       <c r="F201" s="1">
@@ -13082,8 +13079,8 @@
       <c r="D202" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="E202" s="1" t="s">
-        <v>16</v>
+      <c r="E202" t="s">
+        <v>17</v>
       </c>
       <c r="F202" s="1">
         <v>0.25</v>
@@ -13123,8 +13120,8 @@
       <c r="D203" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E203" s="1" t="s">
-        <v>16</v>
+      <c r="E203" t="s">
+        <v>17</v>
       </c>
       <c r="F203" s="1">
         <v>0.25</v>
@@ -13164,8 +13161,8 @@
       <c r="D204" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="E204" s="1" t="s">
-        <v>16</v>
+      <c r="E204" t="s">
+        <v>17</v>
       </c>
       <c r="F204" s="1">
         <v>0.25</v>
@@ -13205,8 +13202,8 @@
       <c r="D205" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="E205" s="1" t="s">
-        <v>16</v>
+      <c r="E205" t="s">
+        <v>17</v>
       </c>
       <c r="F205" s="1">
         <v>0.25</v>
@@ -13246,7 +13243,7 @@
       <c r="D206" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="E206" s="1" t="s">
+      <c r="E206" t="s">
         <v>17</v>
       </c>
       <c r="F206" s="1">
@@ -13287,7 +13284,7 @@
       <c r="D207" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="E207" s="1" t="s">
+      <c r="E207" t="s">
         <v>17</v>
       </c>
       <c r="F207" s="1">
@@ -13328,7 +13325,7 @@
       <c r="D208" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="E208" s="1" t="s">
+      <c r="E208" t="s">
         <v>17</v>
       </c>
       <c r="F208" s="1">
@@ -13369,7 +13366,7 @@
       <c r="D209" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="E209" s="1" t="s">
+      <c r="E209" t="s">
         <v>17</v>
       </c>
       <c r="F209" s="1">
@@ -13410,8 +13407,8 @@
       <c r="D210" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="E210" s="1" t="s">
-        <v>16</v>
+      <c r="E210" t="s">
+        <v>17</v>
       </c>
       <c r="F210" s="1">
         <v>0.25</v>
@@ -13451,8 +13448,8 @@
       <c r="D211" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="E211" s="1" t="s">
-        <v>16</v>
+      <c r="E211" t="s">
+        <v>17</v>
       </c>
       <c r="F211" s="1">
         <v>0.25</v>
@@ -13492,8 +13489,8 @@
       <c r="D212" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="E212" s="1" t="s">
-        <v>16</v>
+      <c r="E212" t="s">
+        <v>17</v>
       </c>
       <c r="F212" s="1">
         <v>0.25</v>
@@ -13533,8 +13530,8 @@
       <c r="D213" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="E213" s="1" t="s">
-        <v>16</v>
+      <c r="E213" t="s">
+        <v>17</v>
       </c>
       <c r="F213" s="1">
         <v>0.25</v>
@@ -13574,7 +13571,7 @@
       <c r="D214" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="E214" s="1" t="s">
+      <c r="E214" t="s">
         <v>17</v>
       </c>
       <c r="F214" s="1">
@@ -13615,7 +13612,7 @@
       <c r="D215" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="E215" s="1" t="s">
+      <c r="E215" t="s">
         <v>17</v>
       </c>
       <c r="F215" s="1">
@@ -13656,7 +13653,7 @@
       <c r="D216" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="E216" s="1" t="s">
+      <c r="E216" t="s">
         <v>17</v>
       </c>
       <c r="F216" s="1">
@@ -13697,7 +13694,7 @@
       <c r="D217" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="E217" s="1" t="s">
+      <c r="E217" t="s">
         <v>17</v>
       </c>
       <c r="F217" s="1">
@@ -13738,8 +13735,8 @@
       <c r="D218" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="E218" s="1" t="s">
-        <v>16</v>
+      <c r="E218" t="s">
+        <v>17</v>
       </c>
       <c r="F218" s="1">
         <v>0.25</v>
@@ -13779,8 +13776,8 @@
       <c r="D219" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="E219" s="1" t="s">
-        <v>16</v>
+      <c r="E219" t="s">
+        <v>17</v>
       </c>
       <c r="F219" s="1">
         <v>0.25</v>
@@ -13820,8 +13817,8 @@
       <c r="D220" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="E220" s="1" t="s">
-        <v>16</v>
+      <c r="E220" t="s">
+        <v>17</v>
       </c>
       <c r="F220" s="1">
         <v>0.25</v>
@@ -13861,8 +13858,8 @@
       <c r="D221" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E221" s="1" t="s">
-        <v>16</v>
+      <c r="E221" t="s">
+        <v>17</v>
       </c>
       <c r="F221" s="1">
         <v>0.25</v>
@@ -13902,7 +13899,7 @@
       <c r="D222" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="E222" s="1" t="s">
+      <c r="E222" t="s">
         <v>17</v>
       </c>
       <c r="F222" s="1">
@@ -13943,7 +13940,7 @@
       <c r="D223" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="E223" s="1" t="s">
+      <c r="E223" t="s">
         <v>17</v>
       </c>
       <c r="F223" s="1">
@@ -13984,7 +13981,7 @@
       <c r="D224" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="E224" s="1" t="s">
+      <c r="E224" t="s">
         <v>17</v>
       </c>
       <c r="F224" s="1">
@@ -14025,7 +14022,7 @@
       <c r="D225" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="E225" s="1" t="s">
+      <c r="E225" t="s">
         <v>17</v>
       </c>
       <c r="F225" s="1">
@@ -14066,8 +14063,8 @@
       <c r="D226" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="E226" s="1" t="s">
-        <v>16</v>
+      <c r="E226" t="s">
+        <v>17</v>
       </c>
       <c r="F226" s="1">
         <v>0.25</v>
@@ -14107,8 +14104,8 @@
       <c r="D227" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="E227" s="1" t="s">
-        <v>16</v>
+      <c r="E227" t="s">
+        <v>17</v>
       </c>
       <c r="F227" s="1">
         <v>0.25</v>
@@ -14148,8 +14145,8 @@
       <c r="D228" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="E228" s="1" t="s">
-        <v>16</v>
+      <c r="E228" t="s">
+        <v>17</v>
       </c>
       <c r="F228" s="1">
         <v>0.25</v>
@@ -14189,8 +14186,8 @@
       <c r="D229" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E229" s="1" t="s">
-        <v>16</v>
+      <c r="E229" t="s">
+        <v>17</v>
       </c>
       <c r="F229" s="1">
         <v>0.25</v>
@@ -14230,7 +14227,7 @@
       <c r="D230" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="E230" s="1" t="s">
+      <c r="E230" t="s">
         <v>17</v>
       </c>
       <c r="F230" s="1">
@@ -14271,7 +14268,7 @@
       <c r="D231" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E231" s="1" t="s">
+      <c r="E231" t="s">
         <v>17</v>
       </c>
       <c r="F231" s="1">
@@ -14312,7 +14309,7 @@
       <c r="D232" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E232" s="1" t="s">
+      <c r="E232" t="s">
         <v>17</v>
       </c>
       <c r="F232" s="1">
@@ -14353,7 +14350,7 @@
       <c r="D233" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="E233" s="1" t="s">
+      <c r="E233" t="s">
         <v>17</v>
       </c>
       <c r="F233" s="1">
@@ -14394,8 +14391,8 @@
       <c r="D234" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="E234" s="1" t="s">
-        <v>16</v>
+      <c r="E234" t="s">
+        <v>17</v>
       </c>
       <c r="F234" s="1">
         <v>0.25</v>
@@ -14435,8 +14432,8 @@
       <c r="D235" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="E235" s="1" t="s">
-        <v>16</v>
+      <c r="E235" t="s">
+        <v>17</v>
       </c>
       <c r="F235" s="1">
         <v>0.25</v>
@@ -14476,8 +14473,8 @@
       <c r="D236" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="E236" s="1" t="s">
-        <v>16</v>
+      <c r="E236" t="s">
+        <v>17</v>
       </c>
       <c r="F236" s="1">
         <v>0.25</v>
@@ -14517,8 +14514,8 @@
       <c r="D237" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="E237" s="1" t="s">
-        <v>16</v>
+      <c r="E237" t="s">
+        <v>17</v>
       </c>
       <c r="F237" s="1">
         <v>0.25</v>
@@ -14558,7 +14555,7 @@
       <c r="D238" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="E238" s="1" t="s">
+      <c r="E238" t="s">
         <v>17</v>
       </c>
       <c r="F238" s="1">
@@ -14599,7 +14596,7 @@
       <c r="D239" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="E239" s="1" t="s">
+      <c r="E239" t="s">
         <v>17</v>
       </c>
       <c r="F239" s="1">
@@ -14640,7 +14637,7 @@
       <c r="D240" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="E240" s="1" t="s">
+      <c r="E240" t="s">
         <v>17</v>
       </c>
       <c r="F240" s="1">
@@ -14681,7 +14678,7 @@
       <c r="D241" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="E241" s="1" t="s">
+      <c r="E241" t="s">
         <v>17</v>
       </c>
       <c r="F241" s="1">
@@ -14722,8 +14719,8 @@
       <c r="D242" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E242" s="1" t="s">
-        <v>16</v>
+      <c r="E242" t="s">
+        <v>17</v>
       </c>
       <c r="F242" s="1">
         <v>0.25</v>
@@ -14763,8 +14760,8 @@
       <c r="D243" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="E243" s="1" t="s">
-        <v>16</v>
+      <c r="E243" t="s">
+        <v>17</v>
       </c>
       <c r="F243" s="1">
         <v>0.25</v>
@@ -14804,8 +14801,8 @@
       <c r="D244" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="E244" s="1" t="s">
-        <v>16</v>
+      <c r="E244" t="s">
+        <v>17</v>
       </c>
       <c r="F244" s="1">
         <v>0.25</v>
@@ -14845,8 +14842,8 @@
       <c r="D245" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="E245" s="1" t="s">
-        <v>16</v>
+      <c r="E245" t="s">
+        <v>17</v>
       </c>
       <c r="F245" s="1">
         <v>0.25</v>
@@ -14886,7 +14883,7 @@
       <c r="D246" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="E246" s="1" t="s">
+      <c r="E246" t="s">
         <v>17</v>
       </c>
       <c r="F246" s="1">
@@ -14927,7 +14924,7 @@
       <c r="D247" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="E247" s="1" t="s">
+      <c r="E247" t="s">
         <v>17</v>
       </c>
       <c r="F247" s="1">
@@ -14968,7 +14965,7 @@
       <c r="D248" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="E248" s="1" t="s">
+      <c r="E248" t="s">
         <v>17</v>
       </c>
       <c r="F248" s="1">
@@ -15009,7 +15006,7 @@
       <c r="D249" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E249" s="1" t="s">
+      <c r="E249" t="s">
         <v>17</v>
       </c>
       <c r="F249" s="1">
@@ -15050,8 +15047,8 @@
       <c r="D250" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="E250" s="1" t="s">
-        <v>16</v>
+      <c r="E250" t="s">
+        <v>17</v>
       </c>
       <c r="F250" s="1">
         <v>0.25</v>
@@ -15091,8 +15088,8 @@
       <c r="D251" s="1" t="s">
         <v>710</v>
       </c>
-      <c r="E251" s="1" t="s">
-        <v>16</v>
+      <c r="E251" t="s">
+        <v>17</v>
       </c>
       <c r="F251" s="1">
         <v>0.25</v>
@@ -15132,8 +15129,8 @@
       <c r="D252" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="E252" s="1" t="s">
-        <v>16</v>
+      <c r="E252" t="s">
+        <v>17</v>
       </c>
       <c r="F252" s="1">
         <v>0.25</v>
@@ -15173,8 +15170,8 @@
       <c r="D253" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E253" s="1" t="s">
-        <v>16</v>
+      <c r="E253" t="s">
+        <v>17</v>
       </c>
       <c r="F253" s="1">
         <v>0.25</v>
@@ -15214,7 +15211,7 @@
       <c r="D254" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="E254" s="1" t="s">
+      <c r="E254" t="s">
         <v>17</v>
       </c>
       <c r="F254" s="1">
@@ -15255,7 +15252,7 @@
       <c r="D255" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E255" s="1" t="s">
+      <c r="E255" t="s">
         <v>17</v>
       </c>
       <c r="F255" s="1">
@@ -15296,7 +15293,7 @@
       <c r="D256" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="E256" s="1" t="s">
+      <c r="E256" t="s">
         <v>17</v>
       </c>
       <c r="F256" s="1">
@@ -15337,7 +15334,7 @@
       <c r="D257" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="E257" s="1" t="s">
+      <c r="E257" t="s">
         <v>17</v>
       </c>
       <c r="F257" s="1">
@@ -15378,8 +15375,8 @@
       <c r="D258" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="E258" s="1" t="s">
-        <v>16</v>
+      <c r="E258" t="s">
+        <v>17</v>
       </c>
       <c r="F258" s="1">
         <v>0.25</v>
@@ -15419,8 +15416,8 @@
       <c r="D259" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="E259" s="1" t="s">
-        <v>16</v>
+      <c r="E259" t="s">
+        <v>17</v>
       </c>
       <c r="F259" s="1">
         <v>0.25</v>
@@ -15460,8 +15457,8 @@
       <c r="D260" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="E260" s="1" t="s">
-        <v>16</v>
+      <c r="E260" t="s">
+        <v>17</v>
       </c>
       <c r="F260" s="1">
         <v>0.25</v>
@@ -15501,8 +15498,8 @@
       <c r="D261" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="E261" s="1" t="s">
-        <v>16</v>
+      <c r="E261" t="s">
+        <v>17</v>
       </c>
       <c r="F261" s="1">
         <v>0.25</v>
@@ -15542,7 +15539,7 @@
       <c r="D262" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="E262" s="1" t="s">
+      <c r="E262" t="s">
         <v>17</v>
       </c>
       <c r="F262" s="1">
@@ -15583,7 +15580,7 @@
       <c r="D263" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="E263" s="1" t="s">
+      <c r="E263" t="s">
         <v>17</v>
       </c>
       <c r="F263" s="1">
@@ -15624,7 +15621,7 @@
       <c r="D264" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="E264" s="1" t="s">
+      <c r="E264" t="s">
         <v>17</v>
       </c>
       <c r="F264" s="1">
@@ -15665,7 +15662,7 @@
       <c r="D265" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="E265" s="1" t="s">
+      <c r="E265" t="s">
         <v>17</v>
       </c>
       <c r="F265" s="1">
@@ -15706,8 +15703,8 @@
       <c r="D266" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="E266" s="1" t="s">
-        <v>16</v>
+      <c r="E266" t="s">
+        <v>17</v>
       </c>
       <c r="F266" s="1">
         <v>0.25</v>
@@ -15747,8 +15744,8 @@
       <c r="D267" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="E267" s="1" t="s">
-        <v>16</v>
+      <c r="E267" t="s">
+        <v>17</v>
       </c>
       <c r="F267" s="1">
         <v>0.25</v>
@@ -15788,8 +15785,8 @@
       <c r="D268" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="E268" s="1" t="s">
-        <v>16</v>
+      <c r="E268" t="s">
+        <v>17</v>
       </c>
       <c r="F268" s="1">
         <v>0.25</v>
@@ -15829,8 +15826,8 @@
       <c r="D269" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="E269" s="1" t="s">
-        <v>16</v>
+      <c r="E269" t="s">
+        <v>17</v>
       </c>
       <c r="F269" s="1">
         <v>0.25</v>
@@ -15870,7 +15867,7 @@
       <c r="D270" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="E270" s="1" t="s">
+      <c r="E270" t="s">
         <v>17</v>
       </c>
       <c r="F270" s="1">
@@ -15911,7 +15908,7 @@
       <c r="D271" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="E271" s="1" t="s">
+      <c r="E271" t="s">
         <v>17</v>
       </c>
       <c r="F271" s="1">
@@ -15952,7 +15949,7 @@
       <c r="D272" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="E272" s="1" t="s">
+      <c r="E272" t="s">
         <v>17</v>
       </c>
       <c r="F272" s="1">
@@ -15993,7 +15990,7 @@
       <c r="D273" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="E273" s="1" t="s">
+      <c r="E273" t="s">
         <v>17</v>
       </c>
       <c r="F273" s="1">
@@ -16034,8 +16031,8 @@
       <c r="D274" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="E274" s="1" t="s">
-        <v>16</v>
+      <c r="E274" t="s">
+        <v>17</v>
       </c>
       <c r="F274" s="1">
         <v>0.25</v>
@@ -16075,8 +16072,8 @@
       <c r="D275" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E275" s="1" t="s">
-        <v>16</v>
+      <c r="E275" t="s">
+        <v>17</v>
       </c>
       <c r="F275" s="1">
         <v>0.25</v>
@@ -16116,8 +16113,8 @@
       <c r="D276" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="E276" s="1" t="s">
-        <v>16</v>
+      <c r="E276" t="s">
+        <v>17</v>
       </c>
       <c r="F276" s="1">
         <v>0.25</v>
@@ -16157,8 +16154,8 @@
       <c r="D277" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="E277" s="1" t="s">
-        <v>16</v>
+      <c r="E277" t="s">
+        <v>17</v>
       </c>
       <c r="F277" s="1">
         <v>0.25</v>
@@ -16198,7 +16195,7 @@
       <c r="D278" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="E278" s="1" t="s">
+      <c r="E278" t="s">
         <v>17</v>
       </c>
       <c r="F278" s="1">
@@ -16239,7 +16236,7 @@
       <c r="D279" s="1" t="s">
         <v>762</v>
       </c>
-      <c r="E279" s="1" t="s">
+      <c r="E279" t="s">
         <v>17</v>
       </c>
       <c r="F279" s="1">
@@ -16280,7 +16277,7 @@
       <c r="D280" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="E280" s="1" t="s">
+      <c r="E280" t="s">
         <v>17</v>
       </c>
       <c r="F280" s="1">
@@ -16321,7 +16318,7 @@
       <c r="D281" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="E281" s="1" t="s">
+      <c r="E281" t="s">
         <v>17</v>
       </c>
       <c r="F281" s="1">
@@ -16362,8 +16359,8 @@
       <c r="D282" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="E282" s="1" t="s">
-        <v>16</v>
+      <c r="E282" t="s">
+        <v>17</v>
       </c>
       <c r="F282" s="1">
         <v>0.25</v>
@@ -16403,8 +16400,8 @@
       <c r="D283" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E283" s="1" t="s">
-        <v>16</v>
+      <c r="E283" t="s">
+        <v>17</v>
       </c>
       <c r="F283" s="1">
         <v>0.25</v>
@@ -16444,8 +16441,8 @@
       <c r="D284" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="E284" s="1" t="s">
-        <v>16</v>
+      <c r="E284" t="s">
+        <v>17</v>
       </c>
       <c r="F284" s="1">
         <v>0.25</v>
@@ -16485,8 +16482,8 @@
       <c r="D285" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="E285" s="1" t="s">
-        <v>16</v>
+      <c r="E285" t="s">
+        <v>17</v>
       </c>
       <c r="F285" s="1">
         <v>0.25</v>
@@ -16526,7 +16523,7 @@
       <c r="D286" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="E286" s="1" t="s">
+      <c r="E286" t="s">
         <v>17</v>
       </c>
       <c r="F286" s="1">
@@ -16567,7 +16564,7 @@
       <c r="D287" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="E287" s="1" t="s">
+      <c r="E287" t="s">
         <v>17</v>
       </c>
       <c r="F287" s="1">
@@ -16608,7 +16605,7 @@
       <c r="D288" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="E288" s="1" t="s">
+      <c r="E288" t="s">
         <v>17</v>
       </c>
       <c r="F288" s="1">
@@ -16649,7 +16646,7 @@
       <c r="D289" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="E289" s="1" t="s">
+      <c r="E289" t="s">
         <v>17</v>
       </c>
       <c r="F289" s="1">
@@ -16690,8 +16687,8 @@
       <c r="D290" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="E290" s="1" t="s">
-        <v>16</v>
+      <c r="E290" t="s">
+        <v>17</v>
       </c>
       <c r="F290" s="1">
         <v>0.25</v>
@@ -16731,8 +16728,8 @@
       <c r="D291" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="E291" s="1" t="s">
-        <v>16</v>
+      <c r="E291" t="s">
+        <v>17</v>
       </c>
       <c r="F291" s="1">
         <v>0.25</v>
@@ -16772,8 +16769,8 @@
       <c r="D292" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="E292" s="1" t="s">
-        <v>16</v>
+      <c r="E292" t="s">
+        <v>17</v>
       </c>
       <c r="F292" s="1">
         <v>0.25</v>
@@ -16813,8 +16810,8 @@
       <c r="D293" s="1" t="s">
         <v>788</v>
       </c>
-      <c r="E293" s="1" t="s">
-        <v>16</v>
+      <c r="E293" t="s">
+        <v>17</v>
       </c>
       <c r="F293" s="1">
         <v>0.25</v>
@@ -16854,7 +16851,7 @@
       <c r="D294" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="E294" s="1" t="s">
+      <c r="E294" t="s">
         <v>17</v>
       </c>
       <c r="F294" s="1">
@@ -16895,7 +16892,7 @@
       <c r="D295" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="E295" s="1" t="s">
+      <c r="E295" t="s">
         <v>17</v>
       </c>
       <c r="F295" s="1">
@@ -16936,7 +16933,7 @@
       <c r="D296" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="E296" s="1" t="s">
+      <c r="E296" t="s">
         <v>17</v>
       </c>
       <c r="F296" s="1">
@@ -16977,7 +16974,7 @@
       <c r="D297" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E297" s="1" t="s">
+      <c r="E297" t="s">
         <v>17</v>
       </c>
       <c r="F297" s="1">
@@ -17018,8 +17015,8 @@
       <c r="D298" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="E298" s="1" t="s">
-        <v>16</v>
+      <c r="E298" t="s">
+        <v>17</v>
       </c>
       <c r="F298" s="1">
         <v>0.25</v>
@@ -17059,8 +17056,8 @@
       <c r="D299" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="E299" s="1" t="s">
-        <v>16</v>
+      <c r="E299" t="s">
+        <v>17</v>
       </c>
       <c r="F299" s="1">
         <v>0.25</v>
@@ -17100,8 +17097,8 @@
       <c r="D300" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E300" s="1" t="s">
-        <v>16</v>
+      <c r="E300" t="s">
+        <v>17</v>
       </c>
       <c r="F300" s="1">
         <v>0.25</v>
@@ -17141,8 +17138,8 @@
       <c r="D301" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E301" s="1" t="s">
-        <v>16</v>
+      <c r="E301" t="s">
+        <v>17</v>
       </c>
       <c r="F301" s="1">
         <v>0.25</v>

</xml_diff>